<commit_message>
Document register has additional columns, including document reference Document reference inserted into all documents Comments on Document Management Policy, and most changes accepted
</commit_message>
<xml_diff>
--- a/OVF.risk_.assessment.xlsx
+++ b/OVF.risk_.assessment.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephreddington/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg.smart\Documents\MHRA-Technical-File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2326DAC-B3E8-DA4A-B7CA-77A5BE92161B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="480" windowWidth="37520" windowHeight="19780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="195" yWindow="480" windowWidth="37515" windowHeight="19785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Risks" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_Hlk264467094" localSheetId="0">Risks!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="74">
   <si>
     <t>What are the hazards?</t>
   </si>
@@ -272,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -721,7 +720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
@@ -729,23 +728,23 @@
       <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="11" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="14" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="2"/>
+    <col min="11" max="11" width="11.140625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="48" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -780,7 +779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="96" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -815,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="65" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -856,7 +855,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -895,7 +894,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -936,7 +935,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -977,7 +976,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="117" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1010,7 +1009,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1043,7 +1042,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1076,7 +1075,7 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1109,7 +1108,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1142,7 +1141,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:16" ht="39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1175,7 +1174,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:16" ht="39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1208,7 +1207,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1241,7 +1240,7 @@
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1274,7 +1273,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:16" ht="39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1307,7 +1306,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1340,7 +1339,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1373,7 +1372,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1406,7 +1405,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1439,7 +1438,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1472,7 +1471,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1505,13 +1504,13 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="13" t="s">
         <v>73</v>
       </c>
@@ -1523,16 +1522,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A917324-0F35-B04A-85D7-992E4E4BD7DF}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>39</v>
       </c>
@@ -1540,13 +1539,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>42</v>
       </c>
@@ -1554,12 +1553,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="8">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>